<commit_message>
math formuls check added but its not working
</commit_message>
<xml_diff>
--- a/Modified Manuscript Sample.xlsx
+++ b/Modified Manuscript Sample.xlsx
@@ -106,7 +106,7 @@
     <t>fuerza gravitacional</t>
   </si>
   <si>
-    <t>fuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetosfuerza de atracción a distancia entre dos objetos</t>
+    <t>fuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetos</t>
   </si>
   <si>
     <t>TXELEM25_gravitationalforce_SP.mp3</t>
@@ -225,9 +225,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -252,6 +252,27 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -260,22 +281,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,8 +336,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,93 +389,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -442,187 +442,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,28 +708,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -745,21 +743,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -783,16 +766,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -805,151 +794,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1228,10 +1228,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1"/>
@@ -1635,6 +1635,12 @@
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
     </row>
+    <row r="14" customHeight="1" spans="5:5">
+      <c r="E14" t="str">
+        <f>_xlfn.CONCAT(E3,E4)</f>
+        <v>equal forces*gravitational force</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Multiple files being downloaded
</commit_message>
<xml_diff>
--- a/Modified Manuscript Sample.xlsx
+++ b/Modified Manuscript Sample.xlsx
@@ -8,13 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="68">
   <si>
     <t>Game Grade</t>
   </si>
@@ -225,10 +227,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -253,9 +255,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -266,8 +268,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -278,6 +281,36 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -320,14 +353,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -336,19 +361,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -361,43 +399,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -442,97 +444,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,85 +618,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,65 +710,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -789,167 +739,219 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -965,8 +967,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,7 +1233,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1"/>
@@ -1276,8 +1278,8 @@
       <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" customHeight="1" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -1304,8 +1306,8 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
     </row>
     <row r="3" customHeight="1" spans="1:14">
       <c r="A3" s="4"/>
@@ -1333,11 +1335,11 @@
       <c r="K3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" customHeight="1" spans="1:14">
       <c r="A4" s="4"/>
@@ -1365,11 +1367,11 @@
       <c r="K4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
     </row>
     <row r="5" customHeight="1" spans="1:14">
       <c r="A5" s="4"/>
@@ -1397,11 +1399,11 @@
       <c r="K5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
     </row>
     <row r="6" customHeight="1" spans="1:14">
       <c r="A6" s="4"/>
@@ -1420,8 +1422,8 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" customHeight="1" spans="1:14">
       <c r="A7" s="4"/>
@@ -1449,11 +1451,11 @@
       <c r="K7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" customHeight="1" spans="1:14">
       <c r="A8" s="4"/>
@@ -1481,11 +1483,11 @@
       <c r="K8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" customHeight="1" spans="1:14">
       <c r="A9" s="4"/>
@@ -1513,11 +1515,11 @@
       <c r="K9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" customHeight="1" spans="1:14">
       <c r="A10" s="4"/>
@@ -1536,8 +1538,8 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" customHeight="1" spans="1:14">
       <c r="A11" s="4"/>
@@ -1565,11 +1567,11 @@
       <c r="K11" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" customHeight="1" spans="1:14">
       <c r="A12" s="4"/>
@@ -1597,11 +1599,11 @@
       <c r="K12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" customHeight="1" spans="1:14">
       <c r="A13" s="4"/>
@@ -1629,13 +1631,830 @@
       <c r="K13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" customHeight="1" spans="5:5">
+      <c r="E14" t="str">
+        <f>_xlfn.CONCAT(E3,E4)</f>
+        <v>equal forces*gravitational force</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="A1:L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="12" max="12" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:14">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:14">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+    </row>
+    <row r="4" customHeight="1" spans="1:14">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+    </row>
+    <row r="5" customHeight="1" spans="1:14">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+    </row>
+    <row r="6" customHeight="1" spans="1:14">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+    </row>
+    <row r="7" customHeight="1" spans="1:14">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:14">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+    </row>
+    <row r="9" customHeight="1" spans="1:14">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+    </row>
+    <row r="10" customHeight="1" spans="1:14">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" customHeight="1" spans="1:14">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" customHeight="1" spans="1:14">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+    </row>
+    <row r="13" customHeight="1" spans="1:14">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+    </row>
+    <row r="14" customHeight="1" spans="5:5">
+      <c r="E14" t="str">
+        <f>_xlfn.CONCAT(E3,E4)</f>
+        <v>equal forces*gravitational force</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="12.5"/>
+  <sheetData>
+    <row r="1" ht="13" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="13" spans="1:12">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" ht="13" spans="1:12">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" ht="13" spans="1:12">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5">
       <c r="E14" t="str">
         <f>_xlfn.CONCAT(E3,E4)</f>
         <v>equal forces*gravitational force</v>

</xml_diff>

<commit_message>
select all button added
</commit_message>
<xml_diff>
--- a/Modified Manuscript Sample.xlsx
+++ b/Modified Manuscript Sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="70">
   <si>
     <t>Game Grade</t>
   </si>
@@ -69,157 +69,163 @@
     <t>Mini-game 1</t>
   </si>
   <si>
+    <t>equal forces</t>
+  </si>
+  <si>
+    <t>forces that have the same strength</t>
+  </si>
+  <si>
+    <t>TXELEM25_equalforces.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_equalforces_def.mp3</t>
+  </si>
+  <si>
+    <t>fuerzas iguales</t>
+  </si>
+  <si>
+    <t>fuerzas que tienen la misma intensidad</t>
+  </si>
+  <si>
+    <t>TXELEM25_equalforces_SP.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_equalforces_def_SP.mp3</t>
+  </si>
+  <si>
+    <t>gravitational force</t>
+  </si>
+  <si>
+    <t>a noncontact force of attraction between two objects</t>
+  </si>
+  <si>
+    <t>TXELEM25_gravitationalforce.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_gravitationalforce_def.mp3</t>
+  </si>
+  <si>
+    <t>fuerza gravitacional</t>
+  </si>
+  <si>
+    <t>fuerza de atraccion a</t>
+  </si>
+  <si>
+    <t>TXELEM25_gravitationalforce_SP.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_gravitationalforce_def_SP.mp3</t>
+  </si>
+  <si>
+    <t>unequal forces</t>
+  </si>
+  <si>
+    <t>forces that have different strengths</t>
+  </si>
+  <si>
+    <t>TXELEM25_unequalforces.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_unequalforces_def.mp3</t>
+  </si>
+  <si>
+    <t>fuerzas desiguales</t>
+  </si>
+  <si>
+    <t>fuerzas que tienen diferentes intensidades</t>
+  </si>
+  <si>
+    <t>TXELEM25_unequalforces_SP.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_unequalforces_def_SP.mp3</t>
+  </si>
+  <si>
+    <t>Mini-game 2</t>
+  </si>
+  <si>
+    <t>potential energy</t>
+  </si>
+  <si>
+    <t>the stored energy an object has</t>
+  </si>
+  <si>
+    <t>TXELEM25_potentialenergy.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_potentialenergy_def.mp3</t>
+  </si>
+  <si>
+    <t>energía potencial</t>
+  </si>
+  <si>
+    <t>energía que un objeto tiene almacenada</t>
+  </si>
+  <si>
+    <t>TXELEM25_potentialenergy_SP.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_potentialenergy_def_SP.mp3</t>
+  </si>
+  <si>
+    <t>frictional force</t>
+  </si>
+  <si>
+    <t>a contact force that pushes against objects in motion</t>
+  </si>
+  <si>
+    <t>TXELEM25_frictionalforce.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_frictionalforce_def.mp3</t>
+  </si>
+  <si>
+    <t>fuerza de fricción</t>
+  </si>
+  <si>
+    <t>fuerza de contacto que empuja en contra de objetos en movimiento</t>
+  </si>
+  <si>
+    <t>TXELEM25_frictionalforce_SP.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_frictionalforce_def_SP.mp3</t>
+  </si>
+  <si>
+    <t>fuerza de atracción a distancia entre dos objetos</t>
+  </si>
+  <si>
+    <t>Mini-game 3</t>
+  </si>
+  <si>
+    <t>kinetic energy</t>
+  </si>
+  <si>
+    <t>the energy an object has due to its motion</t>
+  </si>
+  <si>
+    <t>TXELEM25_kineticenergy.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_kineticenergy_def.mp3</t>
+  </si>
+  <si>
+    <t>energía cinética</t>
+  </si>
+  <si>
+    <t>energía que tiene un cuerpo debido a su movimiento</t>
+  </si>
+  <si>
+    <t>TXELEM25_kineticenergy_SP.mp3</t>
+  </si>
+  <si>
+    <t>TXELEM25_kineticenergy_def_SP.mp3</t>
+  </si>
+  <si>
     <t>equal forces*</t>
   </si>
   <si>
-    <t>forces that have the same strength</t>
-  </si>
-  <si>
-    <t>TXELEM25_equalforces.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_equalforces_def.mp3</t>
-  </si>
-  <si>
-    <t>fuerzas iguales</t>
-  </si>
-  <si>
-    <t>fuerzas que tienen la misma intensidad</t>
-  </si>
-  <si>
-    <t>TXELEM25_equalforces_SP.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_equalforces_def_SP.mp3</t>
-  </si>
-  <si>
-    <t>gravitational force</t>
-  </si>
-  <si>
-    <t>a noncontact force of attraction between two objects</t>
-  </si>
-  <si>
-    <t>TXELEM25_gravitationalforce.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_gravitationalforce_def.mp3</t>
-  </si>
-  <si>
-    <t>fuerza gravitacional</t>
-  </si>
-  <si>
     <t>fuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetosfuerza de atraccion a distancia entre dos objetos</t>
-  </si>
-  <si>
-    <t>TXELEM25_gravitationalforce_SP.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_gravitationalforce_def_SP.mp3</t>
-  </si>
-  <si>
-    <t>unequal forces</t>
-  </si>
-  <si>
-    <t>forces that have different strengths</t>
-  </si>
-  <si>
-    <t>TXELEM25_unequalforces.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_unequalforces_def.mp3</t>
-  </si>
-  <si>
-    <t>fuerzas desiguales</t>
-  </si>
-  <si>
-    <t>fuerzas que tienen diferentes intensidades</t>
-  </si>
-  <si>
-    <t>TXELEM25_unequalforces_SP.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_unequalforces_def_SP.mp3</t>
-  </si>
-  <si>
-    <t>Mini-game 2</t>
-  </si>
-  <si>
-    <t>potential energy</t>
-  </si>
-  <si>
-    <t>the stored energy an object has</t>
-  </si>
-  <si>
-    <t>TXELEM25_potentialenergy.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_potentialenergy_def.mp3</t>
-  </si>
-  <si>
-    <t>energía potencial</t>
-  </si>
-  <si>
-    <t>energía que un objeto tiene almacenada</t>
-  </si>
-  <si>
-    <t>TXELEM25_potentialenergy_SP.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_potentialenergy_def_SP.mp3</t>
-  </si>
-  <si>
-    <t>frictional force</t>
-  </si>
-  <si>
-    <t>a contact force that pushes against objects in motion</t>
-  </si>
-  <si>
-    <t>TXELEM25_frictionalforce.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_frictionalforce_def.mp3</t>
-  </si>
-  <si>
-    <t>fuerza de fricción</t>
-  </si>
-  <si>
-    <t>fuerza de contacto que empuja en contra de objetos en movimiento</t>
-  </si>
-  <si>
-    <t>TXELEM25_frictionalforce_SP.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_frictionalforce_def_SP.mp3</t>
-  </si>
-  <si>
-    <t>fuerza de atracción a distancia entre dos objetos</t>
-  </si>
-  <si>
-    <t>Mini-game 3</t>
-  </si>
-  <si>
-    <t>kinetic energy</t>
-  </si>
-  <si>
-    <t>the energy an object has due to its motion</t>
-  </si>
-  <si>
-    <t>TXELEM25_kineticenergy.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_kineticenergy_def.mp3</t>
-  </si>
-  <si>
-    <t>energía cinética</t>
-  </si>
-  <si>
-    <t>energía que tiene un cuerpo debido a su movimiento</t>
-  </si>
-  <si>
-    <t>TXELEM25_kineticenergy_SP.mp3</t>
-  </si>
-  <si>
-    <t>TXELEM25_kineticenergy_def_SP.mp3</t>
   </si>
 </sst>
 </file>
@@ -1230,10 +1236,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1"/>
@@ -1636,12 +1642,6 @@
       </c>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
-    </row>
-    <row r="14" customHeight="1" spans="5:5">
-      <c r="E14" t="str">
-        <f>_xlfn.CONCAT(E3,E4)</f>
-        <v>equal forces*gravitational force</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1657,7 +1657,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="A1:L14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1"/>
@@ -1739,7 +1739,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>18</v>
@@ -1786,7 +1786,7 @@
         <v>29</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>31</v>
@@ -2154,7 +2154,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>18</v>
@@ -2199,7 +2199,7 @@
         <v>29</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>31</v>

</xml_diff>